<commit_message>
Add ability to schedule a message to be sent in the future
</commit_message>
<xml_diff>
--- a/web/static/templates/httpsms-bulk.xlsx
+++ b/web/static/templates/httpsms-bulk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnold\Work\NdoleStudio\httpsms.com\web\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601B10E-FD8B-4910-BFAA-8D4C0C169158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39AACD5-9325-41EA-9D31-F6CCA14FBB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="4520" windowWidth="38400" windowHeight="15370" xr2:uid="{C835BB88-D79A-4BDE-9D5F-501F78609DA9}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="25780" windowHeight="20880" xr2:uid="{C835BB88-D79A-4BDE-9D5F-501F78609DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>FromPhoneNumber</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>This is a sample text message2</t>
+  </si>
+  <si>
+    <t>SendTime(optional)</t>
+  </si>
+  <si>
+    <t>2023-11-11T02:10:01</t>
   </si>
 </sst>
 </file>
@@ -402,20 +408,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B2B60B-52EE-4979-B69B-CB73D08DD366}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.453125" customWidth="1"/>
     <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="117.36328125" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +432,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>18005550199</v>
       </c>
@@ -437,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>18005550199</v>
       </c>
@@ -446,6 +456,9 @@
       </c>
       <c r="C3" t="s">
         <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>